<commit_message>
Add Transporter information and redetermine source location
</commit_message>
<xml_diff>
--- a/data/호선도크.xlsx
+++ b/data/호선도크.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohyon\PycharmProjects\KSOE-Layout\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohyon\PycharmProjects\Simulation_Module\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98178011-57E0-4066-B3B8-E19D08F0F0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C999EEA3-697F-41E8-B5EF-57873DC94EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="384" windowWidth="10956" windowHeight="16272" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -661,9 +661,9 @@
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -677,7 +677,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -691,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -705,7 +705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -733,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -747,7 +747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -775,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -803,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -817,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -845,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -873,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -901,7 +901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -915,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -929,7 +929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -957,7 +957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -971,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -985,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -1843,7 +1843,7 @@
   <autoFilter ref="A1:D84" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
-        <filter val="2"/>
+        <filter val="1"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>